<commit_message>
Skip if missing name, test.xlsx
</commit_message>
<xml_diff>
--- a/input_files/test.xlsx
+++ b/input_files/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dorian\ExcelToIcs\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED43138-4FBA-414E-94AF-2EB3445DC412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F780EB06-83AF-4075-AA64-A74B629101E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Data</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>Matylda</t>
+  </si>
+  <si>
+    <t>Szkoła</t>
+  </si>
+  <si>
+    <t>Oleszna</t>
+  </si>
+  <si>
+    <t>Przemek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nic </t>
+  </si>
+  <si>
+    <t>Nigdzie</t>
+  </si>
+  <si>
+    <t>Nikt</t>
   </si>
 </sst>
 </file>
@@ -383,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,6 +471,39 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45607</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45547</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>